<commit_message>
Updated the formula for lower AHP scales
</commit_message>
<xml_diff>
--- a/Mapped_AHP_Matrices.xlsx
+++ b/Mapped_AHP_Matrices.xlsx
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="K1" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="L1" t="n">
         <v>1</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
         <v>1</v>
@@ -477,7 +477,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -492,18 +492,18 @@
         <v>2</v>
       </c>
       <c r="K2" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="L2" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -515,7 +515,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="G3" t="n">
         <v>1</v>
@@ -530,59 +530,59 @@
         <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.2</v>
       </c>
       <c r="B4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
         <v>0.25</v>
       </c>
-      <c r="C4" t="n">
+      <c r="G4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="I4" t="n">
         <v>0.25</v>
       </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.1666666666666667</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="J4" t="n">
         <v>0.25</v>
       </c>
-      <c r="H4" t="n">
+      <c r="K4" t="n">
         <v>0.2</v>
       </c>
-      <c r="I4" t="n">
-        <v>0.1666666666666667</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.1666666666666667</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.1428571428571428</v>
-      </c>
       <c r="L4" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -591,30 +591,30 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="K5" t="n">
         <v>0.25</v>
       </c>
-      <c r="I5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.1666666666666667</v>
-      </c>
       <c r="L5" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -644,7 +644,7 @@
         <v>3</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -652,86 +652,86 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
         <v>0.25</v>
       </c>
-      <c r="B7" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.1666666666666667</v>
-      </c>
       <c r="L7" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.2</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="B8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
         <v>0.25</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D8" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.1666666666666667</v>
-      </c>
       <c r="L8" t="n">
-        <v>0.2</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.2</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -743,7 +743,7 @@
         <v>3</v>
       </c>
       <c r="F9" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -758,48 +758,48 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>0.2</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="L9" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
         <v>0.2</v>
       </c>
-      <c r="B10" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="D10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" t="n">
-        <v>3</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="J10" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.1428571428571428</v>
-      </c>
       <c r="L10" t="n">
-        <v>0.2</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="11">
@@ -857,7 +857,7 @@
         <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
         <v>2</v>

</xml_diff>